<commit_message>
[modify] get comment list api
</commit_message>
<xml_diff>
--- a/20.開発/60.API/20.API仕様書/【eternal】API仕様書_Ref003_コメント一覧取得.xlsx
+++ b/20.開発/60.API/20.API仕様書/【eternal】API仕様書_Ref003_コメント一覧取得.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27729"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13880" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="27320" windowHeight="15360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">レスポンス!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'概要(コメント一覧取得)'!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">リクエスト!$A$1:$BV$16</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">レスポンス!$A$1:$BU$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">レスポンス!$A$1:$BV$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'概要(コメント一覧取得)'!$A$1:$BV$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">表紙!$A$1:$AZ$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">変更履歴!$A$1:$F$26</definedName>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="78">
   <si>
     <t>Confidential</t>
     <phoneticPr fontId="6"/>
@@ -510,6 +510,14 @@
   </si>
   <si>
     <t>createDatetime</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>userThumbnailUrl</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ユーザサムネイルURL</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -834,7 +842,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -842,6 +850,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -863,7 +881,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
@@ -1001,6 +1019,45 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1031,6 +1088,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1040,23 +1109,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1067,20 +1121,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="33">
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
@@ -1091,6 +1139,11 @@
     <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="2"/>
@@ -1104,6 +1157,11 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1143,7 +1201,7 @@
         <xdr:cNvPr id="3" name="グループ化 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1162,7 +1220,7 @@
           <xdr:cNvPr id="4" name="正方形/長方形 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1227,7 +1285,7 @@
           <xdr:cNvPr id="5" name="正方形/長方形 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1292,7 +1350,7 @@
           <xdr:cNvPr id="6" name="正方形/長方形 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1357,7 +1415,7 @@
           <xdr:cNvPr id="7" name="正方形/長方形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1422,7 +1480,7 @@
           <xdr:cNvPr id="8" name="正方形/長方形 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1487,7 +1545,7 @@
           <xdr:cNvPr id="9" name="正方形/長方形 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1552,7 +1610,7 @@
           <xdr:cNvPr id="10" name="正方形/長方形 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000A000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1624,7 +1682,7 @@
           <xdr:cNvPr id="11" name="正方形/長方形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000B000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1696,7 +1754,7 @@
           <xdr:cNvPr id="12" name="正方形/長方形 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000C000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1768,7 +1826,7 @@
           <xdr:cNvPr id="13" name="正方形/長方形 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000D000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1840,7 +1898,7 @@
           <xdr:cNvPr id="14" name="正方形/長方形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1912,7 +1970,7 @@
           <xdr:cNvPr id="15" name="正方形/長方形 14">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2005,7 +2063,7 @@
         <xdr:cNvPr id="2" name="グループ化 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4161962-57F9-41FD-BE9B-9C39ABC6F599}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F4161962-57F9-41FD-BE9B-9C39ABC6F599}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2024,7 +2082,7 @@
           <xdr:cNvPr id="3" name="正方形/長方形 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8E14589-EE4C-491D-89A4-EB22863CB61C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A8E14589-EE4C-491D-89A4-EB22863CB61C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2089,7 +2147,7 @@
           <xdr:cNvPr id="4" name="正方形/長方形 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A4FC26D-BF56-4446-B80D-0C5ACFEDC6A5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7A4FC26D-BF56-4446-B80D-0C5ACFEDC6A5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2154,7 +2212,7 @@
           <xdr:cNvPr id="5" name="正方形/長方形 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{118AE21F-A33F-4231-A38E-5951C6EBB37D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{118AE21F-A33F-4231-A38E-5951C6EBB37D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2219,7 +2277,7 @@
           <xdr:cNvPr id="6" name="正方形/長方形 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15CC184C-3B0C-4DA5-8121-88D86F00441F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15CC184C-3B0C-4DA5-8121-88D86F00441F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2284,7 +2342,7 @@
           <xdr:cNvPr id="7" name="正方形/長方形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4754AD5B-2B0B-46EE-8B71-66D219D5EC91}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4754AD5B-2B0B-46EE-8B71-66D219D5EC91}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2349,7 +2407,7 @@
           <xdr:cNvPr id="8" name="正方形/長方形 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C0B29AA-73DD-4127-8070-ABBDAC015AE8}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0C0B29AA-73DD-4127-8070-ABBDAC015AE8}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2414,7 +2472,7 @@
           <xdr:cNvPr id="9" name="正方形/長方形 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E8159FD-54BB-4608-B580-BEF72FA5570A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7E8159FD-54BB-4608-B580-BEF72FA5570A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2486,7 +2544,7 @@
           <xdr:cNvPr id="10" name="正方形/長方形 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB6D827E-0519-43AB-8D27-FC082F456CD0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB6D827E-0519-43AB-8D27-FC082F456CD0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2558,7 +2616,7 @@
           <xdr:cNvPr id="11" name="正方形/長方形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C6F2712-88AD-4AB8-86C6-D7FB58A2F819}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7C6F2712-88AD-4AB8-86C6-D7FB58A2F819}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2630,7 +2688,7 @@
           <xdr:cNvPr id="12" name="正方形/長方形 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15534BB0-4CA1-44E0-A343-8E7681B066C1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15534BB0-4CA1-44E0-A343-8E7681B066C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2702,7 +2760,7 @@
           <xdr:cNvPr id="13" name="正方形/長方形 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFCA127E-94E6-429E-9CA3-34DA0CE0CE72}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CFCA127E-94E6-429E-9CA3-34DA0CE0CE72}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2774,7 +2832,7 @@
           <xdr:cNvPr id="14" name="正方形/長方形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{333B060A-0145-448A-A964-D699A9FE1714}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{333B060A-0145-448A-A964-D699A9FE1714}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2867,7 +2925,7 @@
         <xdr:cNvPr id="2" name="グループ化 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D26842C9-0618-40AE-B87D-E87EF0BA4636}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D26842C9-0618-40AE-B87D-E87EF0BA4636}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2886,7 +2944,7 @@
           <xdr:cNvPr id="3" name="正方形/長方形 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67FBE5C9-53BB-4CF8-8AD1-EB095CBE281F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{67FBE5C9-53BB-4CF8-8AD1-EB095CBE281F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2951,7 +3009,7 @@
           <xdr:cNvPr id="4" name="正方形/長方形 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6BA1B8A-20F1-46E8-94E5-10EC4AEE2D09}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6BA1B8A-20F1-46E8-94E5-10EC4AEE2D09}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3016,7 +3074,7 @@
           <xdr:cNvPr id="5" name="正方形/長方形 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9780BBE8-AC48-4FB7-AAE5-FCCABF1F3CAB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9780BBE8-AC48-4FB7-AAE5-FCCABF1F3CAB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3081,7 +3139,7 @@
           <xdr:cNvPr id="6" name="正方形/長方形 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75E881EB-BDAC-49DC-BC18-62C7AFFF07EB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{75E881EB-BDAC-49DC-BC18-62C7AFFF07EB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3146,7 +3204,7 @@
           <xdr:cNvPr id="7" name="正方形/長方形 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8F811C6-71CA-4EB7-AA95-42C42BEC18E6}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C8F811C6-71CA-4EB7-AA95-42C42BEC18E6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3211,7 +3269,7 @@
           <xdr:cNvPr id="8" name="正方形/長方形 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFC81A55-158C-448F-BC49-95752FE3AC2A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DFC81A55-158C-448F-BC49-95752FE3AC2A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3271,12 +3329,12 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="$BW$3">
+      <xdr:sp macro="" textlink="$BX$3">
         <xdr:nvSpPr>
           <xdr:cNvPr id="9" name="正方形/長方形 8">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E94C7391-D5EA-46A1-90B1-7F7F94EB8CAE}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E94C7391-D5EA-46A1-90B1-7F7F94EB8CAE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3343,12 +3401,12 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="$BX$3">
+      <xdr:sp macro="" textlink="$BY$3">
         <xdr:nvSpPr>
           <xdr:cNvPr id="10" name="正方形/長方形 9">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45A86A5-E097-4C25-966B-43675226397A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D45A86A5-E097-4C25-966B-43675226397A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3415,12 +3473,12 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="$BY$3">
+      <xdr:sp macro="" textlink="$BZ$3">
         <xdr:nvSpPr>
           <xdr:cNvPr id="11" name="正方形/長方形 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15205912-C6AF-458D-B46C-B7B5D8916BEF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{15205912-C6AF-458D-B46C-B7B5D8916BEF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3487,12 +3545,12 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="$BZ$3">
+      <xdr:sp macro="" textlink="$CA$3">
         <xdr:nvSpPr>
           <xdr:cNvPr id="12" name="正方形/長方形 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08AB3292-595D-4F80-888F-88AA0A053D67}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{08AB3292-595D-4F80-888F-88AA0A053D67}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3559,12 +3617,12 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="$CA$3">
+      <xdr:sp macro="" textlink="$CB$3">
         <xdr:nvSpPr>
           <xdr:cNvPr id="13" name="正方形/長方形 12">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E37098A9-4FA1-4543-9354-A3F5552B7C0F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E37098A9-4FA1-4543-9354-A3F5552B7C0F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -3631,12 +3689,12 @@
           </a:p>
         </xdr:txBody>
       </xdr:sp>
-      <xdr:sp macro="" textlink="$CB$3">
+      <xdr:sp macro="" textlink="$CC$3">
         <xdr:nvSpPr>
           <xdr:cNvPr id="14" name="正方形/長方形 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD461C66-31E3-4F1F-A282-33FBF4E7E16F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BD461C66-31E3-4F1F-A282-33FBF4E7E16F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -4047,33 +4105,33 @@
       </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="D12" s="66"/>
+      <c r="D12" s="54"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="52"/>
-      <c r="S13" s="52"/>
-      <c r="T13" s="52"/>
-      <c r="U13" s="52"/>
-      <c r="V13" s="52"/>
-      <c r="W13" s="52"/>
-      <c r="X13" s="52"/>
-      <c r="Y13" s="52"/>
-      <c r="Z13" s="52"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="65"/>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="65"/>
+      <c r="S13" s="65"/>
+      <c r="T13" s="65"/>
+      <c r="U13" s="65"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="65"/>
+      <c r="X13" s="65"/>
+      <c r="Y13" s="65"/>
+      <c r="Z13" s="65"/>
     </row>
     <row r="21" spans="2:51" ht="3" customHeight="1">
       <c r="B21" s="4"/>
@@ -4133,33 +4191,33 @@
       </c>
     </row>
     <row r="27" spans="2:51">
-      <c r="AO27" s="49">
+      <c r="AO27" s="62">
         <f ca="1">INDIRECT("変更履歴!"&amp;LEFT(ADDRESS(ROW(改訂日),COLUMN(改訂日),4,1),1)&amp;COUNTA(改訂日)+4)</f>
         <v>43472</v>
       </c>
-      <c r="AP27" s="50"/>
-      <c r="AQ27" s="50"/>
-      <c r="AR27" s="50"/>
-      <c r="AS27" s="50"/>
-      <c r="AT27" s="50"/>
-      <c r="AU27" s="50"/>
-      <c r="AV27" s="50"/>
-      <c r="AW27" s="50"/>
-      <c r="AX27" s="50"/>
-      <c r="AY27" s="50"/>
+      <c r="AP27" s="63"/>
+      <c r="AQ27" s="63"/>
+      <c r="AR27" s="63"/>
+      <c r="AS27" s="63"/>
+      <c r="AT27" s="63"/>
+      <c r="AU27" s="63"/>
+      <c r="AV27" s="63"/>
+      <c r="AW27" s="63"/>
+      <c r="AX27" s="63"/>
+      <c r="AY27" s="63"/>
     </row>
     <row r="28" spans="2:51">
-      <c r="AR28" s="51" t="str">
+      <c r="AR28" s="64" t="str">
         <f ca="1">INDIRECT("変更履歴!"&amp;LEFT(ADDRESS(ROW(版),COLUMN(版),4,1),1)&amp;COUNTA(版)+4)</f>
         <v>0.0.1</v>
       </c>
-      <c r="AS28" s="51"/>
-      <c r="AT28" s="51"/>
-      <c r="AU28" s="51"/>
-      <c r="AV28" s="51"/>
-      <c r="AW28" s="51"/>
-      <c r="AX28" s="51"/>
-      <c r="AY28" s="51"/>
+      <c r="AS28" s="64"/>
+      <c r="AT28" s="64"/>
+      <c r="AU28" s="64"/>
+      <c r="AV28" s="64"/>
+      <c r="AW28" s="64"/>
+      <c r="AX28" s="64"/>
+      <c r="AY28" s="64"/>
     </row>
     <row r="31" spans="2:51">
       <c r="AR31" s="6"/>
@@ -4203,7 +4261,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="66"/>
+      <c r="A1" s="54"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -4501,13 +4559,13 @@
       <c r="AH11" s="19"/>
     </row>
     <row r="12" spans="2:81" ht="19">
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="55"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="68"/>
       <c r="H12" s="48" t="s">
         <v>57</v>
       </c>
@@ -4796,67 +4854,67 @@
       </c>
     </row>
     <row r="9" spans="2:81">
-      <c r="C9" s="56">
+      <c r="C9" s="69">
         <f>ROW()-ROW($C$8)</f>
         <v>1</v>
       </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56" t="s">
+      <c r="D9" s="69"/>
+      <c r="E9" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56" t="s">
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="M9" s="56"/>
-      <c r="N9" s="56"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="56" t="s">
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="T9" s="56"/>
-      <c r="U9" s="56"/>
-      <c r="V9" s="56"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="56"/>
-      <c r="Y9" s="56"/>
-      <c r="Z9" s="56" t="s">
+      <c r="T9" s="69"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="69"/>
+      <c r="W9" s="69"/>
+      <c r="X9" s="69"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="AA9" s="56"/>
-      <c r="AB9" s="56"/>
-      <c r="AC9" s="56"/>
-      <c r="AD9" s="56"/>
-      <c r="AE9" s="56"/>
-      <c r="AF9" s="56"/>
-      <c r="AG9" s="57" t="s">
+      <c r="AA9" s="69"/>
+      <c r="AB9" s="69"/>
+      <c r="AC9" s="69"/>
+      <c r="AD9" s="69"/>
+      <c r="AE9" s="69"/>
+      <c r="AF9" s="69"/>
+      <c r="AG9" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="AH9" s="57"/>
-      <c r="AI9" s="58"/>
-      <c r="AJ9" s="58"/>
-      <c r="AK9" s="58"/>
-      <c r="AL9" s="58"/>
-      <c r="AM9" s="58"/>
-      <c r="AN9" s="58"/>
-      <c r="AO9" s="58"/>
-      <c r="AP9" s="58"/>
-      <c r="AQ9" s="58"/>
-      <c r="AR9" s="58"/>
-      <c r="AS9" s="58"/>
-      <c r="AT9" s="58"/>
-      <c r="AU9" s="58"/>
-      <c r="AV9" s="58"/>
-      <c r="AW9" s="58"/>
-      <c r="AX9" s="58"/>
+      <c r="AH9" s="70"/>
+      <c r="AI9" s="71"/>
+      <c r="AJ9" s="71"/>
+      <c r="AK9" s="71"/>
+      <c r="AL9" s="71"/>
+      <c r="AM9" s="71"/>
+      <c r="AN9" s="71"/>
+      <c r="AO9" s="71"/>
+      <c r="AP9" s="71"/>
+      <c r="AQ9" s="71"/>
+      <c r="AR9" s="71"/>
+      <c r="AS9" s="71"/>
+      <c r="AT9" s="71"/>
+      <c r="AU9" s="71"/>
+      <c r="AV9" s="71"/>
+      <c r="AW9" s="71"/>
+      <c r="AX9" s="71"/>
       <c r="BX9" s="9" t="s">
         <v>31</v>
       </c>
@@ -4865,69 +4923,69 @@
       </c>
     </row>
     <row r="10" spans="2:81" ht="19" customHeight="1">
-      <c r="C10" s="56">
+      <c r="C10" s="69">
         <f>ROW()-ROW($C$8)</f>
         <v>2</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56" t="s">
+      <c r="D10" s="69"/>
+      <c r="E10" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56" t="s">
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="56" t="s">
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="T10" s="56"/>
-      <c r="U10" s="56"/>
-      <c r="V10" s="56"/>
-      <c r="W10" s="56"/>
-      <c r="X10" s="56"/>
-      <c r="Y10" s="56"/>
-      <c r="Z10" s="56" t="s">
+      <c r="T10" s="69"/>
+      <c r="U10" s="69"/>
+      <c r="V10" s="69"/>
+      <c r="W10" s="69"/>
+      <c r="X10" s="69"/>
+      <c r="Y10" s="69"/>
+      <c r="Z10" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="AA10" s="56"/>
-      <c r="AB10" s="56"/>
-      <c r="AC10" s="56"/>
-      <c r="AD10" s="56"/>
-      <c r="AE10" s="56"/>
-      <c r="AF10" s="56"/>
-      <c r="AG10" s="57" t="s">
+      <c r="AA10" s="69"/>
+      <c r="AB10" s="69"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="69"/>
+      <c r="AE10" s="69"/>
+      <c r="AF10" s="69"/>
+      <c r="AG10" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="AH10" s="57"/>
-      <c r="AI10" s="58" t="s">
+      <c r="AH10" s="70"/>
+      <c r="AI10" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="AJ10" s="58"/>
-      <c r="AK10" s="58"/>
-      <c r="AL10" s="58"/>
-      <c r="AM10" s="58"/>
-      <c r="AN10" s="58"/>
-      <c r="AO10" s="58"/>
-      <c r="AP10" s="58"/>
-      <c r="AQ10" s="58"/>
-      <c r="AR10" s="58"/>
-      <c r="AS10" s="58"/>
-      <c r="AT10" s="58"/>
-      <c r="AU10" s="58"/>
-      <c r="AV10" s="58"/>
-      <c r="AW10" s="58"/>
-      <c r="AX10" s="58"/>
+      <c r="AJ10" s="71"/>
+      <c r="AK10" s="71"/>
+      <c r="AL10" s="71"/>
+      <c r="AM10" s="71"/>
+      <c r="AN10" s="71"/>
+      <c r="AO10" s="71"/>
+      <c r="AP10" s="71"/>
+      <c r="AQ10" s="71"/>
+      <c r="AR10" s="71"/>
+      <c r="AS10" s="71"/>
+      <c r="AT10" s="71"/>
+      <c r="AU10" s="71"/>
+      <c r="AV10" s="71"/>
+      <c r="AW10" s="71"/>
+      <c r="AX10" s="71"/>
       <c r="BX10" s="9" t="s">
         <v>42</v>
       </c>
@@ -5010,64 +5068,65 @@
       <c r="AX13" s="19"/>
     </row>
     <row r="14" spans="2:81">
-      <c r="C14" s="56" t="s">
+      <c r="C14" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="56"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="56"/>
-      <c r="S14" s="56"/>
-      <c r="T14" s="56"/>
-      <c r="U14" s="56"/>
-      <c r="V14" s="56"/>
-      <c r="W14" s="56"/>
-      <c r="X14" s="56"/>
-      <c r="Y14" s="56"/>
-      <c r="Z14" s="56"/>
-      <c r="AA14" s="56"/>
-      <c r="AB14" s="56"/>
-      <c r="AC14" s="56"/>
-      <c r="AD14" s="56"/>
-      <c r="AE14" s="56"/>
-      <c r="AF14" s="56"/>
-      <c r="AG14" s="57"/>
-      <c r="AH14" s="57"/>
-      <c r="AI14" s="58"/>
-      <c r="AJ14" s="58"/>
-      <c r="AK14" s="58"/>
-      <c r="AL14" s="58"/>
-      <c r="AM14" s="58"/>
-      <c r="AN14" s="58"/>
-      <c r="AO14" s="58"/>
-      <c r="AP14" s="58"/>
-      <c r="AQ14" s="58"/>
-      <c r="AR14" s="58"/>
-      <c r="AS14" s="58"/>
-      <c r="AT14" s="58"/>
-      <c r="AU14" s="58"/>
-      <c r="AV14" s="58"/>
-      <c r="AW14" s="58"/>
-      <c r="AX14" s="58"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="69"/>
+      <c r="Q14" s="69"/>
+      <c r="R14" s="69"/>
+      <c r="S14" s="69"/>
+      <c r="T14" s="69"/>
+      <c r="U14" s="69"/>
+      <c r="V14" s="69"/>
+      <c r="W14" s="69"/>
+      <c r="X14" s="69"/>
+      <c r="Y14" s="69"/>
+      <c r="Z14" s="69"/>
+      <c r="AA14" s="69"/>
+      <c r="AB14" s="69"/>
+      <c r="AC14" s="69"/>
+      <c r="AD14" s="69"/>
+      <c r="AE14" s="69"/>
+      <c r="AF14" s="69"/>
+      <c r="AG14" s="70"/>
+      <c r="AH14" s="70"/>
+      <c r="AI14" s="71"/>
+      <c r="AJ14" s="71"/>
+      <c r="AK14" s="71"/>
+      <c r="AL14" s="71"/>
+      <c r="AM14" s="71"/>
+      <c r="AN14" s="71"/>
+      <c r="AO14" s="71"/>
+      <c r="AP14" s="71"/>
+      <c r="AQ14" s="71"/>
+      <c r="AR14" s="71"/>
+      <c r="AS14" s="71"/>
+      <c r="AT14" s="71"/>
+      <c r="AU14" s="71"/>
+      <c r="AV14" s="71"/>
+      <c r="AW14" s="71"/>
+      <c r="AX14" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:K14"/>
-    <mergeCell ref="L14:R14"/>
-    <mergeCell ref="S14:Y14"/>
-    <mergeCell ref="Z14:AF14"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:K9"/>
+    <mergeCell ref="L9:R9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:K10"/>
+    <mergeCell ref="L10:R10"/>
     <mergeCell ref="AG14:AH14"/>
     <mergeCell ref="AI14:AX14"/>
     <mergeCell ref="S9:Y9"/>
@@ -5078,12 +5137,11 @@
     <mergeCell ref="Z10:AF10"/>
     <mergeCell ref="AG10:AH10"/>
     <mergeCell ref="AI10:AX10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:K9"/>
-    <mergeCell ref="L9:R9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:K10"/>
-    <mergeCell ref="L10:R10"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:K14"/>
+    <mergeCell ref="L14:R14"/>
+    <mergeCell ref="S14:Y14"/>
+    <mergeCell ref="Z14:AF14"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="1">
@@ -5107,82 +5165,82 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:CB42"/>
+  <dimension ref="B1:CC42"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="3.125" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="0.875" style="9" customWidth="1"/>
-    <col min="2" max="73" width="3.125" style="9" customWidth="1"/>
-    <col min="74" max="74" width="3.125" style="9"/>
-    <col min="75" max="81" width="8.625" style="9" customWidth="1"/>
-    <col min="82" max="16384" width="3.125" style="9"/>
+    <col min="2" max="74" width="3.125" style="9" customWidth="1"/>
+    <col min="75" max="75" width="3.125" style="9"/>
+    <col min="76" max="82" width="8.625" style="9" customWidth="1"/>
+    <col min="83" max="16384" width="3.125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:80" ht="6.75" customHeight="1"/>
-    <row r="2" spans="2:80">
-      <c r="BW2" s="10" t="s">
+    <row r="1" spans="2:81" ht="6.75" customHeight="1"/>
+    <row r="2" spans="2:81">
+      <c r="BX2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="BX2" s="10" t="s">
+      <c r="BY2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="BY2" s="10" t="s">
+      <c r="BZ2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="BZ2" s="10" t="s">
+      <c r="CA2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="CA2" s="10" t="s">
+      <c r="CB2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="CB2" s="10" t="s">
+      <c r="CC2" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:80">
-      <c r="BW3" s="10" t="s">
+    <row r="3" spans="2:81">
+      <c r="BX3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="BX3" s="9" t="str">
+      <c r="BY3" s="9" t="str">
         <f ca="1">REPLACE(LEFT(CELL("filename",$A$1),FIND(".x",CELL("filename",$A$1))-1),1,FIND("[",CELL("filename",$A$1)),)</f>
         <v>【eternal】API仕様書_Ref003_コメント一覧取得</v>
       </c>
-      <c r="BY3" s="11">
+      <c r="BZ3" s="11">
         <v>43434</v>
       </c>
-      <c r="BZ3" s="10" t="s">
+      <c r="CA3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="CA3" s="11">
+      <c r="CB3" s="11">
         <v>43467</v>
       </c>
-      <c r="CB3" s="10" t="s">
+      <c r="CC3" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:80" ht="18" customHeight="1"/>
-    <row r="6" spans="2:80">
+    <row r="4" spans="2:81" ht="18" customHeight="1"/>
+    <row r="6" spans="2:81">
       <c r="B6" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:80">
+    <row r="7" spans="2:81">
       <c r="C7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="BW7" s="9" t="s">
+      <c r="BX7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="BZ7" s="9" t="s">
+      <c r="CA7" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:80">
+    <row r="8" spans="2:81">
       <c r="C8" s="26" t="s">
         <v>23</v>
       </c>
@@ -5227,10 +5285,10 @@
       <c r="AH8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="AI8" s="18" t="s">
+      <c r="AI8" s="19"/>
+      <c r="AJ8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="AJ8" s="24"/>
       <c r="AK8" s="24"/>
       <c r="AL8" s="24"/>
       <c r="AM8" s="24"/>
@@ -5244,153 +5302,156 @@
       <c r="AU8" s="24"/>
       <c r="AV8" s="24"/>
       <c r="AW8" s="24"/>
-      <c r="AX8" s="19"/>
-      <c r="BW8" s="9" t="s">
+      <c r="AX8" s="24"/>
+      <c r="AY8" s="19"/>
+      <c r="BX8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="BZ8" s="9" t="s">
+      <c r="CA8" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:80">
+    <row r="9" spans="2:81">
       <c r="C9" s="29">
         <v>1</v>
       </c>
       <c r="D9" s="30"/>
       <c r="E9" s="31"/>
-      <c r="F9" s="63" t="s">
+      <c r="F9" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="63" t="s">
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="65" t="s">
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="73"/>
+      <c r="R9" s="73"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="U9" s="65"/>
-      <c r="V9" s="65"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="65"/>
-      <c r="Y9" s="65"/>
-      <c r="Z9" s="65"/>
-      <c r="AA9" s="65" t="s">
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
+      <c r="X9" s="75"/>
+      <c r="Y9" s="75"/>
+      <c r="Z9" s="75"/>
+      <c r="AA9" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="AB9" s="65"/>
-      <c r="AC9" s="65"/>
-      <c r="AD9" s="65"/>
-      <c r="AE9" s="65"/>
-      <c r="AF9" s="65"/>
-      <c r="AG9" s="65"/>
-      <c r="AH9" s="67" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI9" s="62"/>
-      <c r="AJ9" s="62"/>
-      <c r="AK9" s="62"/>
-      <c r="AL9" s="62"/>
-      <c r="AM9" s="62"/>
-      <c r="AN9" s="62"/>
-      <c r="AO9" s="62"/>
-      <c r="AP9" s="62"/>
-      <c r="AQ9" s="62"/>
-      <c r="AR9" s="62"/>
-      <c r="AS9" s="62"/>
-      <c r="AT9" s="62"/>
-      <c r="AU9" s="62"/>
-      <c r="AV9" s="62"/>
-      <c r="AW9" s="62"/>
-      <c r="AX9" s="62"/>
-      <c r="BW9" s="9" t="s">
+      <c r="AB9" s="75"/>
+      <c r="AC9" s="75"/>
+      <c r="AD9" s="75"/>
+      <c r="AE9" s="75"/>
+      <c r="AF9" s="75"/>
+      <c r="AG9" s="75"/>
+      <c r="AH9" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI9" s="84"/>
+      <c r="AJ9" s="72"/>
+      <c r="AK9" s="72"/>
+      <c r="AL9" s="72"/>
+      <c r="AM9" s="72"/>
+      <c r="AN9" s="72"/>
+      <c r="AO9" s="72"/>
+      <c r="AP9" s="72"/>
+      <c r="AQ9" s="72"/>
+      <c r="AR9" s="72"/>
+      <c r="AS9" s="72"/>
+      <c r="AT9" s="72"/>
+      <c r="AU9" s="72"/>
+      <c r="AV9" s="72"/>
+      <c r="AW9" s="72"/>
+      <c r="AX9" s="72"/>
+      <c r="AY9" s="72"/>
+      <c r="BX9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="BZ9" s="9" t="s">
+      <c r="CA9" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:80">
+    <row r="10" spans="2:81">
       <c r="C10" s="32"/>
       <c r="D10" s="33">
         <v>2</v>
       </c>
       <c r="E10" s="31"/>
-      <c r="F10" s="71" t="s">
+      <c r="F10" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="71" t="s">
+      <c r="G10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="63"/>
-      <c r="O10" s="63"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="63"/>
-      <c r="R10" s="63"/>
-      <c r="S10" s="64"/>
-      <c r="T10" s="68" t="s">
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+      <c r="R10" s="73"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="U10" s="69"/>
-      <c r="V10" s="69"/>
-      <c r="W10" s="69"/>
-      <c r="X10" s="69"/>
-      <c r="Y10" s="69"/>
-      <c r="Z10" s="70"/>
-      <c r="AA10" s="68" t="s">
+      <c r="U10" s="81"/>
+      <c r="V10" s="81"/>
+      <c r="W10" s="81"/>
+      <c r="X10" s="81"/>
+      <c r="Y10" s="81"/>
+      <c r="Z10" s="82"/>
+      <c r="AA10" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="AB10" s="69"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="69"/>
-      <c r="AE10" s="69"/>
-      <c r="AF10" s="69"/>
-      <c r="AG10" s="70"/>
-      <c r="AH10" s="67" t="s">
+      <c r="AB10" s="81"/>
+      <c r="AC10" s="81"/>
+      <c r="AD10" s="81"/>
+      <c r="AE10" s="81"/>
+      <c r="AF10" s="81"/>
+      <c r="AG10" s="82"/>
+      <c r="AH10" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="AI10" s="59"/>
-      <c r="AJ10" s="60"/>
-      <c r="AK10" s="60"/>
-      <c r="AL10" s="60"/>
-      <c r="AM10" s="60"/>
-      <c r="AN10" s="60"/>
-      <c r="AO10" s="60"/>
-      <c r="AP10" s="60"/>
-      <c r="AQ10" s="60"/>
-      <c r="AR10" s="60"/>
-      <c r="AS10" s="60"/>
-      <c r="AT10" s="60"/>
-      <c r="AU10" s="60"/>
-      <c r="AV10" s="60"/>
-      <c r="AW10" s="60"/>
-      <c r="AX10" s="61"/>
-      <c r="BW10" s="9" t="s">
+      <c r="AI10" s="84"/>
+      <c r="AJ10" s="76"/>
+      <c r="AK10" s="77"/>
+      <c r="AL10" s="77"/>
+      <c r="AM10" s="77"/>
+      <c r="AN10" s="77"/>
+      <c r="AO10" s="77"/>
+      <c r="AP10" s="77"/>
+      <c r="AQ10" s="77"/>
+      <c r="AR10" s="77"/>
+      <c r="AS10" s="77"/>
+      <c r="AT10" s="77"/>
+      <c r="AU10" s="77"/>
+      <c r="AV10" s="77"/>
+      <c r="AW10" s="77"/>
+      <c r="AX10" s="77"/>
+      <c r="AY10" s="78"/>
+      <c r="BX10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="BZ10" s="9" t="s">
+      <c r="CA10" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:80">
-      <c r="C11" s="73"/>
-      <c r="D11" s="72">
+    <row r="11" spans="2:81">
+      <c r="C11" s="60"/>
+      <c r="D11" s="59">
         <v>4</v>
       </c>
       <c r="E11" s="25"/>
@@ -5430,11 +5491,11 @@
       <c r="AE11" s="46"/>
       <c r="AF11" s="46"/>
       <c r="AG11" s="47"/>
-      <c r="AH11" s="67" t="s">
+      <c r="AH11" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="AI11" s="39"/>
-      <c r="AJ11" s="40"/>
+      <c r="AI11" s="84"/>
+      <c r="AJ11" s="39"/>
       <c r="AK11" s="40"/>
       <c r="AL11" s="40"/>
       <c r="AM11" s="40"/>
@@ -5448,17 +5509,18 @@
       <c r="AU11" s="40"/>
       <c r="AV11" s="40"/>
       <c r="AW11" s="40"/>
-      <c r="AX11" s="41"/>
-      <c r="BW11" s="9" t="s">
+      <c r="AX11" s="40"/>
+      <c r="AY11" s="41"/>
+      <c r="BX11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="BZ11" s="9" t="s">
+      <c r="CA11" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:80">
-      <c r="C12" s="73"/>
-      <c r="D12" s="72">
+    <row r="12" spans="2:81">
+      <c r="C12" s="60"/>
+      <c r="D12" s="59">
         <v>5</v>
       </c>
       <c r="E12" s="25"/>
@@ -5498,11 +5560,11 @@
       <c r="AE12" s="46"/>
       <c r="AF12" s="46"/>
       <c r="AG12" s="47"/>
-      <c r="AH12" s="67" t="s">
+      <c r="AH12" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="AI12" s="39"/>
-      <c r="AJ12" s="40"/>
+      <c r="AI12" s="84"/>
+      <c r="AJ12" s="39"/>
       <c r="AK12" s="40"/>
       <c r="AL12" s="40"/>
       <c r="AM12" s="40"/>
@@ -5516,19 +5578,20 @@
       <c r="AU12" s="40"/>
       <c r="AV12" s="40"/>
       <c r="AW12" s="40"/>
-      <c r="AX12" s="41"/>
-      <c r="BZ12" s="9" t="s">
+      <c r="AX12" s="40"/>
+      <c r="AY12" s="41"/>
+      <c r="CA12" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:80">
-      <c r="C13" s="74"/>
-      <c r="D13" s="72">
+    <row r="13" spans="2:81">
+      <c r="C13" s="60"/>
+      <c r="D13" s="59">
         <v>6</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G13" s="42"/>
       <c r="H13" s="42"/>
@@ -5537,7 +5600,7 @@
       <c r="K13" s="42"/>
       <c r="L13" s="43"/>
       <c r="M13" s="44" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="N13" s="42"/>
       <c r="O13" s="42"/>
@@ -5563,11 +5626,11 @@
       <c r="AE13" s="46"/>
       <c r="AF13" s="46"/>
       <c r="AG13" s="47"/>
-      <c r="AH13" s="67" t="s">
+      <c r="AH13" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="AI13" s="39"/>
-      <c r="AJ13" s="40"/>
+      <c r="AI13" s="84"/>
+      <c r="AJ13" s="39"/>
       <c r="AK13" s="40"/>
       <c r="AL13" s="40"/>
       <c r="AM13" s="40"/>
@@ -5581,28 +5644,101 @@
       <c r="AU13" s="40"/>
       <c r="AV13" s="40"/>
       <c r="AW13" s="40"/>
-      <c r="AX13" s="41"/>
-      <c r="BZ13" s="9" t="s">
+      <c r="AX13" s="40"/>
+      <c r="AY13" s="41"/>
+      <c r="CA13" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:81">
+      <c r="C14" s="61"/>
+      <c r="D14" s="59">
+        <v>7</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="U14" s="56"/>
+      <c r="V14" s="56"/>
+      <c r="W14" s="56"/>
+      <c r="X14" s="56"/>
+      <c r="Y14" s="56"/>
+      <c r="Z14" s="57"/>
+      <c r="AA14" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB14" s="56"/>
+      <c r="AC14" s="56"/>
+      <c r="AD14" s="56"/>
+      <c r="AE14" s="56"/>
+      <c r="AF14" s="56"/>
+      <c r="AG14" s="57"/>
+      <c r="AH14" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI14" s="84"/>
+      <c r="AJ14" s="49"/>
+      <c r="AK14" s="50"/>
+      <c r="AL14" s="50"/>
+      <c r="AM14" s="50"/>
+      <c r="AN14" s="50"/>
+      <c r="AO14" s="50"/>
+      <c r="AP14" s="50"/>
+      <c r="AQ14" s="50"/>
+      <c r="AR14" s="50"/>
+      <c r="AS14" s="50"/>
+      <c r="AT14" s="50"/>
+      <c r="AU14" s="50"/>
+      <c r="AV14" s="50"/>
+      <c r="AW14" s="50"/>
+      <c r="AX14" s="50"/>
+      <c r="AY14" s="51"/>
+      <c r="CA14" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="42" ht="19" customHeight="1"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="AI9:AX9"/>
+  <mergeCells count="16">
+    <mergeCell ref="AH14:AI14"/>
+    <mergeCell ref="AH10:AI10"/>
+    <mergeCell ref="AH11:AI11"/>
+    <mergeCell ref="AH12:AI12"/>
+    <mergeCell ref="AH13:AI13"/>
+    <mergeCell ref="AJ10:AY10"/>
+    <mergeCell ref="F10:L10"/>
+    <mergeCell ref="M10:S10"/>
+    <mergeCell ref="T10:Z10"/>
+    <mergeCell ref="AA10:AG10"/>
+    <mergeCell ref="AJ9:AY9"/>
     <mergeCell ref="F9:L9"/>
     <mergeCell ref="M9:S9"/>
     <mergeCell ref="T9:Z9"/>
     <mergeCell ref="AA9:AG9"/>
-    <mergeCell ref="AI10:AX10"/>
-    <mergeCell ref="F10:L10"/>
-    <mergeCell ref="M10:S10"/>
-    <mergeCell ref="T10:Z10"/>
-    <mergeCell ref="AA10:AG10"/>
+    <mergeCell ref="AH9:AI9"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH9:AH13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI9 AH9:AH14">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>